<commit_message>
Update excel with Jenkins
</commit_message>
<xml_diff>
--- a/DataID.xlsx
+++ b/DataID.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4060" yWindow="3460" windowWidth="20240" windowHeight="17960" tabRatio="500"/>
+    <workbookView xWindow="11700" yWindow="8680" windowWidth="20240" windowHeight="17960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Login Info" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>URL:</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>Jenkins:</t>
   </si>
 </sst>
 </file>
@@ -471,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -484,7 +487,7 @@
     <col min="4" max="4" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -497,8 +500,11 @@
       <c r="D1" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -511,32 +517,35 @@
       <c r="D2" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>

</xml_diff>